<commit_message>
new file and changes
</commit_message>
<xml_diff>
--- a/01ComparacionesArticulo2.xlsx
+++ b/01ComparacionesArticulo2.xlsx
@@ -491,7 +491,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>83.11029815323103</t>
+          <t>83.1102981641134</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -506,7 +506,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-476.85244136181313</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -528,7 +528,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>400.0000000652878</t>
+          <t>400.0000000176049</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -543,7 +543,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-462.8409244919828</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -565,7 +565,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>399.99999997111746</t>
+          <t>400.0000000356312</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -580,7 +580,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-390.2720508695672</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -602,7 +602,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>420.0000001243805</t>
+          <t>420.0000000374189</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -617,7 +617,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-486.8191586029397</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -654,7 +654,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-138.22243104805233</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -676,7 +676,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>388.49548200218254</t>
+          <t>358.07549512951493</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -691,7 +691,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>37.49204221702779</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -713,7 +713,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>299.37177172947554</t>
+          <t>299.3835951197538</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -728,7 +728,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-119.60442139538192</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -750,7 +750,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>400.00000010462</t>
+          <t>400.0000000410847</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -787,7 +787,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>400.0000001046187</t>
+          <t>400.00000004108404</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -802,12 +802,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>675.7517231211192</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>956.0920837703245</t>
+          <t>796.7433714822</t>
         </is>
       </c>
     </row>
@@ -824,7 +824,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>400.0000001033924</t>
+          <t>400.00000004041436</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -839,7 +839,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1264.0717322700705</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -861,7 +861,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>400.0000001049183</t>
+          <t>400.0000000412478</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -876,7 +876,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1124.264125978972</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -898,7 +898,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>400.00000010462</t>
+          <t>400.0000000410847</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -913,7 +913,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>800.37976258646</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -935,7 +935,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>400.0000001049183</t>
+          <t>400.0000000412478</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -950,7 +950,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-18.858220925469503</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -972,7 +972,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>489.6205959022451</t>
+          <t>489.62065399352576</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -987,7 +987,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>959.0322788555521</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1009,7 +1009,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>400.00000025108733</t>
+          <t>400.0000001247187</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>400.00000025108733</t>
+          <t>400.0000001247187</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1083,7 +1083,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>400.00000025099104</t>
+          <t>400.0000001250004</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1098,7 +1098,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>253.87520101539747</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1120,7 +1120,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>400.0000002510867</t>
+          <t>400.00000012471844</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1135,7 +1135,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-581.1465953978322</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -1157,7 +1157,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>472.79419472957835</t>
+          <t>500.0</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1172,7 +1172,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-0.019818332195148107</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -1194,7 +1194,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>170.39999398946387</t>
+          <t>170.39999387651875</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1209,7 +1209,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-299.487372693519</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>400.00000022075903</t>
+          <t>400.00000011271607</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1246,7 +1246,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-732.4069906486361</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -1268,7 +1268,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>400.0000002395249</t>
+          <t>400.000000119644</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1283,7 +1283,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-806.047954553181</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -1305,7 +1305,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>400.0000004932788</t>
+          <t>399.99999994878533</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1320,7 +1320,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-501.27656027536034</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -1342,7 +1342,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>420.00000022297763</t>
+          <t>420.00000009118696</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-138.22243104805236</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -1379,7 +1379,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>489.6200329355156</t>
+          <t>489.6201370111077</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1416,7 +1416,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>400.0000002395249</t>
+          <t>400.000000119644</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -1431,7 +1431,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-119.60442139538192</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -1475,7 +1475,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>58.94824951638855</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -1519,7 +1519,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-62.48896717923746</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -1541,7 +1541,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-62.48896717923779</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -1563,7 +1563,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>203.2570807097871</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -1585,7 +1585,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>203.25708070978746</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -1607,7 +1607,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>44.3725497239757</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
@@ -1629,7 +1629,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>44.37254972397571</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -1707,7 +1707,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>83.11029815323103</t>
+          <t>83.1102981641134</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -1722,7 +1722,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-438.27835994496365</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -1759,7 +1759,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-462.80828808309724</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -1781,7 +1781,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>399.99999997111746</t>
+          <t>400.0000000356312</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -1796,7 +1796,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-389.44181835079087</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -1818,7 +1818,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>420.0000001243805</t>
+          <t>420.0000000374189</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -1833,7 +1833,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-486.8009536421274</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -1855,7 +1855,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>456.76055491974006</t>
+          <t>456.7606477280851</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -1870,7 +1870,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-119.07707149006714</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -1892,7 +1892,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>299.9117434894461</t>
+          <t>298.9999999997249</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -1907,7 +1907,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>37.557303398225415</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -1929,7 +1929,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>299.37177172947554</t>
+          <t>299.3835951197538</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -1944,7 +1944,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-119.1950950003588</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1966,7 +1966,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>400.00000010462</t>
+          <t>400.0000000410847</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -2003,7 +2003,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>400.0000001046187</t>
+          <t>400.00000004108404</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -2018,12 +2018,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>694.268708738456</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>956.0920837703245</t>
+          <t>796.7433714822</t>
         </is>
       </c>
     </row>
@@ -2040,7 +2040,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>400.0000001033924</t>
+          <t>400.00000004041436</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -2055,7 +2055,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1264.336978268255</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -2077,7 +2077,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>400.0000001049183</t>
+          <t>400.0000000412478</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -2092,7 +2092,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1125.5689278971631</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -2114,7 +2114,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>400.00000010462</t>
+          <t>400.0000000410847</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -2129,7 +2129,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>800.3900951422893</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -2151,7 +2151,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>400.0000001049183</t>
+          <t>400.0000000412478</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -2188,7 +2188,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>491.75248607398953</t>
+          <t>491.7523107815771</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -2203,7 +2203,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>959.2364766498399</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -2225,7 +2225,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>400.00000025108733</t>
+          <t>400.0000001247187</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -2262,7 +2262,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>400.00000025108733</t>
+          <t>400.0000001247187</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -2277,7 +2277,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-35.768021113128384</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -2299,7 +2299,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>400.00000025099104</t>
+          <t>400.0000001250004</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -2314,7 +2314,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>253.94594162461001</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -2336,7 +2336,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>400.0000002510867</t>
+          <t>400.00000012471844</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -2351,7 +2351,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-579.7841364209398</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -2373,7 +2373,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>500.0</t>
+          <t>497.78327147087157</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -2388,7 +2388,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-0.025255159646968898</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -2410,7 +2410,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>170.39999398946387</t>
+          <t>170.39999387651875</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -2425,7 +2425,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-335.3871663101083</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -2447,7 +2447,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>400.00000022075903</t>
+          <t>400.00000011271607</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -2462,7 +2462,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-732.4391777331941</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -2484,7 +2484,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>400.0000002395249</t>
+          <t>400.000000119644</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -2499,7 +2499,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-806.8760812053656</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>400.0000004932788</t>
+          <t>399.99999994878533</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -2536,7 +2536,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-501.2947652361671</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -2558,7 +2558,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>420.00000022297763</t>
+          <t>420.00000009118696</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -2573,7 +2573,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-119.07707149006718</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -2595,7 +2595,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>491.75115107478734</t>
+          <t>491.75177291206927</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -2632,7 +2632,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>400.0000002395249</t>
+          <t>400.000000119644</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -2647,7 +2647,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-119.1950950003588</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -2691,7 +2691,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>31.639467094110003</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -2713,7 +2713,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>31.639467094109992</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -2735,7 +2735,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-63.828026465895995</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -2757,7 +2757,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-63.82802646589035</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -2779,7 +2779,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>204.55163692264557</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -2801,7 +2801,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>204.55163692264594</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -2823,7 +2823,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>45.43150729770366</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
@@ -2845,7 +2845,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>45.431507297703654</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -2923,7 +2923,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>83.11029815323103</t>
+          <t>83.1102981641134</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -2938,7 +2938,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-43.459327353400724</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -2960,7 +2960,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>400.0000000652878</t>
+          <t>400.0000000176049</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -2975,7 +2975,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-462.8898979642314</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -2997,7 +2997,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>399.99999997111746</t>
+          <t>400.0000000356312</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -3012,7 +3012,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-390.88486197237575</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -3034,7 +3034,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>420.0000001243805</t>
+          <t>420.0000000374189</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -3049,7 +3049,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-486.9553120373505</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -3071,7 +3071,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>452.2201932083481</t>
+          <t>452.22080960748644</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -3086,7 +3086,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>77.98291472269224</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -3108,7 +3108,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>307.1208638138918</t>
+          <t>298.9999999997249</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -3123,7 +3123,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-3.752525846700998e-05</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -3160,7 +3160,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-119.95826046392548</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -3182,7 +3182,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>400.00000010462</t>
+          <t>400.0000000410847</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -3197,7 +3197,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>9.631388136617925</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -3219,7 +3219,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>400.0000001046187</t>
+          <t>400.00000004108404</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -3234,12 +3234,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>695.7389085759012</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>956.0920837703245</t>
+          <t>796.7433714822</t>
         </is>
       </c>
     </row>
@@ -3256,7 +3256,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>400.0000001033924</t>
+          <t>400.00000004041436</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -3271,7 +3271,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1263.6777624668707</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -3293,7 +3293,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>400.0000001049183</t>
+          <t>400.0000000412478</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -3308,7 +3308,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1122.5789147601035</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -3330,7 +3330,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>400.00000010462</t>
+          <t>400.0000000410847</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -3345,7 +3345,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>799.8954017744701</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -3367,7 +3367,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>400.0000001049183</t>
+          <t>400.0000000412478</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -3404,7 +3404,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>487.21600180974826</t>
+          <t>487.2166134412663</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -3419,7 +3419,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>958.7280351725541</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -3441,7 +3441,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>400.00000025108733</t>
+          <t>400.0000001247187</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -3456,7 +3456,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-0.1583245037458638</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -3478,7 +3478,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>400.00000025108733</t>
+          <t>400.0000001247187</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -3493,7 +3493,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-348.78939788391824</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -3515,7 +3515,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>400.00000025099104</t>
+          <t>400.0000001250004</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -3530,7 +3530,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>253.7652409305541</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -3552,7 +3552,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>400.0000002510867</t>
+          <t>400.00000012471844</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -3567,7 +3567,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-581.8224010630845</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -3589,7 +3589,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>400.00000025099104</t>
+          <t>411.58897700967134</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -3626,7 +3626,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>170.39999398946387</t>
+          <t>170.39999387651875</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -3641,7 +3641,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-649.6806607976703</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -3663,7 +3663,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>400.00000022075903</t>
+          <t>400.00000011271607</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -3678,7 +3678,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-732.3586913433825</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -3700,7 +3700,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>400.0000002395249</t>
+          <t>400.000000119644</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -3715,7 +3715,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-805.4366978323034</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -3737,7 +3737,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>400.0000004932788</t>
+          <t>399.99999994878533</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -3752,7 +3752,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-501.1404068406879</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -3774,7 +3774,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>420.00000022297763</t>
+          <t>420.00000009118696</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -3789,7 +3789,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>77.98291472269227</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -3811,7 +3811,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>487.215141288055</t>
+          <t>487.2157974776127</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -3826,7 +3826,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>37.39270553515247</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -3848,7 +3848,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>400.0000002395249</t>
+          <t>400.000000119644</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -3863,7 +3863,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-119.95826046392548</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -3907,7 +3907,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>46.592598269624354</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -3951,7 +3951,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-103.59666999025876</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -3973,7 +3973,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-103.59666999025876</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -3995,7 +3995,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>248.12815062631546</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -4017,7 +4017,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>248.12815062631594</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -4039,7 +4039,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>38.59861173073795</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
@@ -4061,7 +4061,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>38.598611730738355</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -4139,7 +4139,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>83.11029815323103</t>
+          <t>83.1102981641134</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -4154,7 +4154,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-200.02805901586385</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -4176,7 +4176,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>400.0000000652878</t>
+          <t>400.0000000176049</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -4191,7 +4191,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-188.72741634293783</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -4213,7 +4213,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>399.99999997111746</t>
+          <t>400.0000000356312</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -4228,7 +4228,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-390.3225852764998</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -4250,7 +4250,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>420.0000001243805</t>
+          <t>420.0000000374189</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -4265,7 +4265,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-488.61484594877106</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -4287,7 +4287,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>454.56031195550014</t>
+          <t>396.7433828793597</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -4324,7 +4324,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>333.80019343645165</t>
+          <t>308.9473409650441</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -4339,7 +4339,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>148.18953600778673</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -4361,7 +4361,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>299.37177172947554</t>
+          <t>299.3835951197538</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -4376,7 +4376,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-119.62521800637376</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -4398,7 +4398,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>400.00000010462</t>
+          <t>400.0000000410847</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>79.5455848850956</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -4435,7 +4435,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>400.0000001046187</t>
+          <t>400.00000004108404</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -4450,12 +4450,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>796.3941013969464</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>956.0920837703245</t>
+          <t>796.7433714822</t>
         </is>
       </c>
     </row>
@@ -4472,7 +4472,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>400.0000001033924</t>
+          <t>400.00000004041436</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -4487,7 +4487,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1332.2403989625527</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -4509,7 +4509,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>400.0000001049183</t>
+          <t>400.0000000412478</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -4524,7 +4524,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1124.2458387738018</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -4546,7 +4546,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>400.00000010462</t>
+          <t>400.0000000410847</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -4561,7 +4561,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>795.7007037537583</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -4583,7 +4583,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>400.0000001049183</t>
+          <t>400.0000000412478</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -4598,7 +4598,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>96.39559408059051</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -4620,7 +4620,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>489.55939666807177</t>
+          <t>489.5607066648654</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -4635,7 +4635,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1034.3929433734363</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -4657,7 +4657,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>400.00000025108733</t>
+          <t>400.0000001247187</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -4672,7 +4672,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-1.8282474118247276</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -4709,7 +4709,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-91.22133875848775</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -4731,7 +4731,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>400.00000025099104</t>
+          <t>400.0000001250004</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -4746,7 +4746,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>347.8940392377415</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -4768,7 +4768,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>400.0000002510867</t>
+          <t>400.00000012471844</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -4783,7 +4783,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-581.2579688043515</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -4805,7 +4805,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>400.00000025099104</t>
+          <t>500.0</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -4842,7 +4842,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>170.39999398946387</t>
+          <t>170.39999387651875</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -4857,7 +4857,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-391.8033047288304</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -4879,7 +4879,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>400.00000022075903</t>
+          <t>400.00000011271607</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -4894,7 +4894,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-607.9835232735547</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -4916,7 +4916,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>400.0000002395249</t>
+          <t>400.000000119644</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -4931,7 +4931,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-805.997548325663</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -4953,7 +4953,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>400.0000004932788</t>
+          <t>399.99999994878533</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -4968,7 +4968,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-499.48087292952425</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -4990,7 +4990,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>420.00000022297763</t>
+          <t>420.00000009118696</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -5005,7 +5005,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.139651416505324e-05</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -5027,7 +5027,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>489.5674823003413</t>
+          <t>489.5687839147222</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -5042,7 +5042,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>148.18953600778673</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -5064,7 +5064,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>400.0000002395249</t>
+          <t>400.000000119644</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -5079,7 +5079,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-119.62521800637376</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -5101,7 +5101,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>79.54558488509558</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -5123,7 +5123,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-95.97132749109326</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -5167,7 +5167,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-154.32492248856872</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -5189,7 +5189,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-154.32492248856872</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -5211,7 +5211,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>371.560017721006</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -5233,7 +5233,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>371.5600177210063</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -5255,7 +5255,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-32.965799263576045</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
@@ -5277,7 +5277,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-32.965799263576045</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -5355,7 +5355,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>83.11029815323103</t>
+          <t>83.1102981641134</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -5370,7 +5370,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-44.8992741717568</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -5392,7 +5392,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>400.0000000652878</t>
+          <t>400.0000000176049</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -5407,7 +5407,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-468.3658101196141</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -5429,7 +5429,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>399.99999997111746</t>
+          <t>400.0000000356312</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -5444,7 +5444,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-389.9585527545011</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -5466,7 +5466,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>420.0000001243805</t>
+          <t>420.0000000374189</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -5481,7 +5481,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-488.8470349463189</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -5503,7 +5503,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>455.4418592750254</t>
+          <t>455.44341753259465</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -5518,7 +5518,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>77.5734253890989</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -5540,7 +5540,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>306.133392929617</t>
+          <t>298.9999999997249</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -5555,7 +5555,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>26.115655347194654</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -5577,7 +5577,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>299.37177172947554</t>
+          <t>299.3835951197538</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -5592,7 +5592,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-119.44871549219265</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -5614,7 +5614,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>400.00000010462</t>
+          <t>400.0000000410847</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -5629,7 +5629,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>84.20643664574385</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -5651,7 +5651,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>400.0000001046187</t>
+          <t>400.00000004108404</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -5666,12 +5666,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>699.7787403043855</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>956.0920837703245</t>
+          <t>796.7433714822</t>
         </is>
       </c>
     </row>
@@ -5688,7 +5688,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>400.0000001033924</t>
+          <t>400.00000004041436</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -5703,7 +5703,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1221.426143416667</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -5725,7 +5725,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>400.0000001049183</t>
+          <t>400.0000000412478</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -5740,7 +5740,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1124.7715720294748</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -5762,7 +5762,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>400.00000010462</t>
+          <t>400.0000000410847</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -5777,7 +5777,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>795.0711089750715</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -5799,7 +5799,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>400.0000001049183</t>
+          <t>400.0000000412478</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -5814,7 +5814,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>9.351550134491621e-05</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -5836,7 +5836,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>490.4410774160259</t>
+          <t>490.442712809505</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -5851,7 +5851,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>925.9076053495214</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -5873,7 +5873,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>400.00000025108733</t>
+          <t>400.0000001247187</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -5888,7 +5888,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-2.0784941312163503</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -5910,7 +5910,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>400.00000025108733</t>
+          <t>400.0000001247187</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -5925,7 +5925,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-204.36078886408015</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -5962,7 +5962,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>240.61113024225654</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -5984,7 +5984,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>400.0000002510867</t>
+          <t>400.00000012471844</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -5999,7 +5999,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-580.6386903821603</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -6021,7 +6021,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>443.8001463022035</t>
+          <t>471.16514429229125</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -6058,7 +6058,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>170.39999398946387</t>
+          <t>170.39999387651875</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -6073,7 +6073,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-505.5129240445194</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -6095,7 +6095,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>400.00000022075903</t>
+          <t>400.00000011271607</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -6110,7 +6110,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-726.9581639266507</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -6132,7 +6132,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>400.0000002395249</t>
+          <t>400.000000119644</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -6147,7 +6147,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-806.360657487145</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -6169,7 +6169,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>400.0000004932788</t>
+          <t>399.99999994878533</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -6184,7 +6184,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-499.2486839319266</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -6206,7 +6206,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>420.00000022297763</t>
+          <t>420.00000009118696</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -6221,7 +6221,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>77.5734253890976</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -6243,7 +6243,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>490.44978964729967</t>
+          <t>490.45148875204603</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -6280,7 +6280,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>400.0000002395249</t>
+          <t>400.000000119644</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -6295,7 +6295,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-119.44871549219265</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -6317,7 +6317,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>84.20643664574385</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -6339,7 +6339,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-51.38099751579956</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -6361,7 +6361,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-51.38099751579956</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -6383,7 +6383,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-174.6723369079266</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -6405,7 +6405,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-174.67233690792656</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -6427,7 +6427,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>395.7167707360286</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -6449,7 +6449,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>395.7167707360287</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -6471,7 +6471,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-36.883906624453886</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
@@ -6493,7 +6493,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-36.88390662445388</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -6571,7 +6571,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>83.11029815323103</t>
+          <t>83.1102981641134</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -6586,7 +6586,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-43.455798537492015</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -6608,7 +6608,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>400.0000000652878</t>
+          <t>400.0000000176049</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -6623,7 +6623,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-462.7978105465429</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -6645,7 +6645,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>399.99999997111746</t>
+          <t>400.0000000356312</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -6660,7 +6660,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-541.1365909704335</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -6682,7 +6682,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>420.0000001243805</t>
+          <t>420.0000000374189</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -6697,7 +6697,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-436.82553705328877</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -6719,7 +6719,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>457.14272341695835</t>
+          <t>457.1425904034508</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -6734,7 +6734,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>78.38586389296611</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -6756,7 +6756,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>304.8387232076102</t>
+          <t>307.1591138469874</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -6771,7 +6771,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>37.57857936718954</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -6793,7 +6793,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>299.37177172947554</t>
+          <t>299.3835951197538</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -6808,7 +6808,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-194.7014873295867</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -6830,7 +6830,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>400.00000010462</t>
+          <t>400.0000000410847</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -6867,7 +6867,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>400.0000001046187</t>
+          <t>400.00000004108404</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -6882,12 +6882,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>699.8503895156998</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>956.0920837703245</t>
+          <t>796.7433714822</t>
         </is>
       </c>
     </row>
@@ -6919,7 +6919,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1264.4204343226447</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -6941,7 +6941,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>400.0000001049183</t>
+          <t>400.0000000412478</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -6956,7 +6956,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>878.0615007629301</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -6978,7 +6978,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>400.00000010462</t>
+          <t>400.0000000410847</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -6993,7 +6993,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>750.622473841529</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -7015,7 +7015,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>400.0000001049183</t>
+          <t>400.0000000412478</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -7052,7 +7052,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>492.15366854354414</t>
+          <t>492.1535966624448</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -7067,7 +7067,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>959.3009700570339</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -7089,7 +7089,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>400.00000025108733</t>
+          <t>400.0000001247187</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -7104,7 +7104,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-49.67016039426136</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -7126,7 +7126,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>400.00000025108733</t>
+          <t>400.0000001247187</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -7141,7 +7141,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-333.02251388099353</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -7163,7 +7163,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>400.00000025099104</t>
+          <t>400.0000001250004</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -7178,7 +7178,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>253.9697685109613</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -7200,7 +7200,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>400.0000002510867</t>
+          <t>400.00000012471844</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -7215,7 +7215,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-824.6962847956155</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -7252,7 +7252,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-49.760060786513996</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -7274,7 +7274,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>170.39999398946387</t>
+          <t>170.39999387651875</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -7289,7 +7289,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-635.363972920083</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -7311,7 +7311,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>400.00000022075903</t>
+          <t>400.00000011271607</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -7326,7 +7326,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-732.4495110296849</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -7348,7 +7348,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>400.0000002395249</t>
+          <t>400.000000119644</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -7363,7 +7363,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-655.5660790526186</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -7385,7 +7385,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>400.0000004932788</t>
+          <t>399.99999994878533</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -7400,7 +7400,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-551.2701818250248</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -7422,7 +7422,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>420.00000022297763</t>
+          <t>420.00000009118696</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -7437,7 +7437,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>78.38586389296617</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -7459,7 +7459,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>492.14328421012004</t>
+          <t>492.1431057592792</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -7496,7 +7496,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>400.0000002395249</t>
+          <t>400.000000119644</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -7511,7 +7511,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-194.70148732959808</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -7533,7 +7533,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-45.54430471680575</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -7555,7 +7555,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-119.49404641389964</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -7577,7 +7577,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-119.49404641389962</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -7599,7 +7599,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-110.75109843305171</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -7621,7 +7621,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-110.75109843305171</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -7643,7 +7643,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>203.4786096279871</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -7665,7 +7665,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>203.47860962798728</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -7687,7 +7687,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>93.12605090606183</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
@@ -7709,7 +7709,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>93.1260509060618</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -7787,7 +7787,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>83.11029815323103</t>
+          <t>83.1102981641134</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -7802,7 +7802,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-200.17285119375558</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -7824,7 +7824,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>400.0000000652878</t>
+          <t>400.0000000176049</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -7839,7 +7839,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-462.9180432847205</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -7861,7 +7861,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>399.99999997111746</t>
+          <t>400.0000000356312</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -7876,7 +7876,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-389.53312898750676</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -7898,7 +7898,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>420.0000001243805</t>
+          <t>420.0000000374189</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -7913,7 +7913,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-217.1338208954108</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -7935,7 +7935,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>456.8232884091876</t>
+          <t>396.7433714646718</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -7972,7 +7972,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>303.99823137379354</t>
+          <t>361.0749511408736</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -8009,7 +8009,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>299.37177172947554</t>
+          <t>299.3835951197538</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -8024,7 +8024,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-119.22099286304184</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -8046,7 +8046,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>400.00000010462</t>
+          <t>400.0000000410847</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -8083,7 +8083,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>400.0000001046187</t>
+          <t>400.00000004108404</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -8098,12 +8098,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>796.3941013969464</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>956.0920837703245</t>
+          <t>796.7433714822</t>
         </is>
       </c>
     </row>
@@ -8120,7 +8120,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>400.0000001033924</t>
+          <t>400.00000004041436</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -8135,7 +8135,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1263.4892597416108</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -8157,7 +8157,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>400.0000001049183</t>
+          <t>400.0000000412478</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -8172,7 +8172,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1125.6969459480988</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -8194,7 +8194,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>400.00000010462</t>
+          <t>400.0000000410847</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -8209,7 +8209,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>924.8714505300187</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -8231,7 +8231,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>400.0000001049183</t>
+          <t>400.0000000412478</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -8246,7 +8246,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>96.14590786913759</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -8268,7 +8268,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>491.8226006245122</t>
+          <t>491.82954861820764</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -8283,7 +8283,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>958.5780049385015</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -8305,7 +8305,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>400.00000025108733</t>
+          <t>400.0000001247187</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -8320,7 +8320,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>125.61235673704185</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -8342,7 +8342,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>400.00000025108733</t>
+          <t>400.0000001247187</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -8357,7 +8357,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-84.50830206920877</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -8379,7 +8379,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>400.00000025099104</t>
+          <t>400.0000001250004</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -8394,7 +8394,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>253.68208029388555</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -8416,7 +8416,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>400.0000002510867</t>
+          <t>400.00000012471844</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -8431,7 +8431,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-580.0586547098526</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -8468,7 +8468,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>126.60289474404493</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -8490,7 +8490,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>170.39999398946387</t>
+          <t>170.39999387651875</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -8505,7 +8505,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-385.26448161475287</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -8527,7 +8527,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>400.00000022075903</t>
+          <t>400.00000011271607</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -8542,7 +8542,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-732.3309334884935</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -8564,7 +8564,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>400.0000002395249</t>
+          <t>400.000000119644</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -8579,7 +8579,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-806.7850021760776</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -8616,7 +8616,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-372.3030611317588</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -8638,7 +8638,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>420.00000022297763</t>
+          <t>420.00000009118696</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -8675,7 +8675,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>491.8295169062344</t>
+          <t>491.8359989661517</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -8690,7 +8690,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>37.33103371373209</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -8712,7 +8712,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>400.0000002395249</t>
+          <t>400.000000119644</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -8727,7 +8727,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-119.22099286304184</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -8749,7 +8749,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>78.88041297218238</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -8771,7 +8771,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-70.46312705073609</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -8793,7 +8793,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-70.46312705073609</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -8815,7 +8815,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-157.49641525530498</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -8837,7 +8837,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-157.49641525530498</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -8859,7 +8859,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>202.8786633189661</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -8881,7 +8881,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>202.87866331896646</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -8903,7 +8903,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-56.346568442022885</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
@@ -8925,7 +8925,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-56.34656844202289</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -9003,7 +9003,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>83.11029815323103</t>
+          <t>83.1102981641134</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -9018,7 +9018,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-43.76604388854654</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -9040,7 +9040,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>400.0000000652878</t>
+          <t>400.0000000176049</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -9055,7 +9055,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-462.8605050175178</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -9077,7 +9077,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>399.99999997111746</t>
+          <t>400.0000000356312</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -9092,7 +9092,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-389.3696336080531</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -9114,7 +9114,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>420.0000001243805</t>
+          <t>420.0000000374189</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -9129,7 +9129,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-404.198895308477</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -9151,7 +9151,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>457.0538309927043</t>
+          <t>457.0661199811953</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -9166,7 +9166,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>78.23974826787152</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -9188,7 +9188,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>390.9512911179283</t>
+          <t>304.7895961264533</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -9203,7 +9203,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>37.449797108514815</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -9225,7 +9225,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>299.37177172947554</t>
+          <t>299.3835951197538</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -9240,7 +9240,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-119.15139987898395</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -9262,7 +9262,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>400.00000010462</t>
+          <t>400.0000000410847</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -9277,7 +9277,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-98.59411179717806</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -9299,7 +9299,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>400.0000001046187</t>
+          <t>400.00000004108404</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -9314,12 +9314,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>700.066452836654</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>956.0920837703245</t>
+          <t>796.7433714822</t>
         </is>
       </c>
     </row>
@@ -9336,7 +9336,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>400.0000001033924</t>
+          <t>400.00000004041436</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -9351,7 +9351,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1263.936199157161</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -9373,7 +9373,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>400.0000001049183</t>
+          <t>400.0000000412478</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -9388,7 +9388,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1125.7950304517337</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -9410,7 +9410,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>400.00000010462</t>
+          <t>400.0000000410847</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -9425,7 +9425,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>714.0676772664089</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -9447,7 +9447,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>400.0000001049183</t>
+          <t>400.0000000412478</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -9484,7 +9484,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>492.0566899033605</t>
+          <t>492.0673117782611</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -9499,7 +9499,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>958.9250499505918</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -9521,7 +9521,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>400.00000025108733</t>
+          <t>400.0000001247187</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -9536,7 +9536,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-83.94099201703399</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -9558,7 +9558,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>400.00000025108733</t>
+          <t>400.0000001247187</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -9573,7 +9573,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-247.86327821077228</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -9595,7 +9595,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>400.00000025099104</t>
+          <t>400.0000001250004</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -9610,7 +9610,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>253.81990997037437</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -9632,7 +9632,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>400.0000002510867</t>
+          <t>400.00000012471844</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -9647,7 +9647,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-579.717058598511</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -9669,7 +9669,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>413.0488934870849</t>
+          <t>500.0</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -9684,7 +9684,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-82.87517660503312</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -9706,7 +9706,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>170.39999398946387</t>
+          <t>170.39999387651875</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -9721,7 +9721,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-549.5287560536098</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -9758,7 +9758,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-732.3876796489341</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -9780,7 +9780,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>400.0000002395249</t>
+          <t>400.000000119644</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -9795,7 +9795,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-806.9480828530834</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -9817,7 +9817,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>400.0000004932788</t>
+          <t>399.99999994878533</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -9832,7 +9832,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-583.8855436010215</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -9854,7 +9854,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>420.00000022297763</t>
+          <t>420.00000009118696</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -9869,7 +9869,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>78.2397482678715</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -9891,7 +9891,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>492.06257404620726</t>
+          <t>492.0750428452021</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -9928,7 +9928,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>400.0000002395249</t>
+          <t>400.000000119644</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -9943,7 +9943,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-119.15139987898398</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -9987,7 +9987,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-75.85131140530805</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -10009,7 +10009,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-75.85131140530805</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -10031,7 +10031,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-153.40200364548582</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -10053,7 +10053,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-153.4020036454986</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -10075,7 +10075,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>203.16659535495685</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -10097,7 +10097,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>203.1665953549572</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -10119,7 +10119,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-62.017703835741536</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
@@ -10141,7 +10141,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-62.017703835741536</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -10219,7 +10219,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>83.11029815323103</t>
+          <t>83.1102981641134</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -10256,7 +10256,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>400.0000000652878</t>
+          <t>400.0000000176049</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -10271,7 +10271,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-463.0886366549243</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -10293,7 +10293,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>399.99999997111746</t>
+          <t>400.0000000356312</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -10308,7 +10308,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-389.67697253383494</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -10330,7 +10330,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>420.0000001243805</t>
+          <t>420.0000000374189</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -10345,7 +10345,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-261.5957845235898</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -10367,7 +10367,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>455.41860358163825</t>
+          <t>455.40363784850354</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -10382,7 +10382,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>100.0473134066576</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -10404,7 +10404,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>298.9999999935089</t>
+          <t>333.74967258498094</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -10441,7 +10441,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>299.37177172947554</t>
+          <t>299.3835951197538</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -10456,7 +10456,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-119.35724061259066</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -10478,7 +10478,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>400.00000010462</t>
+          <t>400.0000000410847</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -10515,7 +10515,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>400.0000001046187</t>
+          <t>400.00000004108404</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -10530,12 +10530,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>654.7535952677578</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>956.0920837703245</t>
+          <t>796.7433714822</t>
         </is>
       </c>
     </row>
@@ -10552,7 +10552,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>400.0000001033924</t>
+          <t>400.00000004041436</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -10567,7 +10567,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1262.1643523836742</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -10589,7 +10589,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>400.0000001049183</t>
+          <t>400.0000000412478</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -10604,7 +10604,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1124.5523333067279</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -10626,7 +10626,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>400.00000010462</t>
+          <t>400.0000000410847</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -10641,7 +10641,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>939.9893068077228</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -10663,7 +10663,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>400.0000001049183</t>
+          <t>400.0000000412478</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -10678,7 +10678,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-44.916430386998826</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -10700,7 +10700,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>490.4190734845092</t>
+          <t>490.40453435910837</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -10715,7 +10715,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>957.5504434202403</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -10737,7 +10737,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>400.00000025108733</t>
+          <t>400.0000001247187</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -10752,7 +10752,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>151.03782733273124</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -10774,7 +10774,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>400.00000025108733</t>
+          <t>400.0000001247187</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -10789,7 +10789,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-251.1920171128559</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -10811,7 +10811,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>400.00000025099104</t>
+          <t>400.0000001250004</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -10826,7 +10826,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>253.2785196352818</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -10848,7 +10848,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>400.0000002510867</t>
+          <t>400.00000012471844</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -10863,7 +10863,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-579.8742404133734</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -10885,7 +10885,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>470.50440673132636</t>
+          <t>500.0</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -10900,7 +10900,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-230.71222905433567</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -10922,7 +10922,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>170.39999398946387</t>
+          <t>170.39999387651875</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -10937,7 +10937,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-552.6173380860047</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -10959,7 +10959,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>400.00000022075903</t>
+          <t>400.00000011271607</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -10974,7 +10974,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-732.1626886104333</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -11011,7 +11011,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-806.6415234857512</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -11033,7 +11033,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>400.0000004932788</t>
+          <t>399.99999994878533</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -11048,7 +11048,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-726.055595930467</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -11070,7 +11070,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>420.00000022297763</t>
+          <t>420.00000009118696</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -11085,7 +11085,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>100.04731340665762</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -11107,7 +11107,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>490.4300108742117</t>
+          <t>429.2542886853422</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -11122,7 +11122,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>36.98169615132633</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -11144,7 +11144,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>400.0000002395249</t>
+          <t>400.000000119644</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -11159,7 +11159,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-119.35724061259066</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -11203,7 +11203,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-139.3797113007853</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -11247,7 +11247,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-173.52200328373493</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -11269,7 +11269,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-173.52200328373493</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -11291,7 +11291,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>202.02650413115003</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -11313,7 +11313,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>202.02650413115043</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -11357,7 +11357,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-111.52426486321238</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">

</xml_diff>